<commit_message>
Update format of cardlist
</commit_message>
<xml_diff>
--- a/Game Design/CardList.xlsx
+++ b/Game Design/CardList.xlsx
@@ -5,14 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Or\Documents\EAE 3710\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\UGrimoire\Grimoire\Game Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="4650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="4650" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Master" sheetId="1" r:id="rId1"/>
+    <sheet name="Tier 1" sheetId="2" r:id="rId2"/>
+    <sheet name="Tier 2" sheetId="3" r:id="rId3"/>
+    <sheet name="Tier 3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="49">
   <si>
     <t>Card Name</t>
   </si>
@@ -135,13 +138,49 @@
   </si>
   <si>
     <t>#</t>
+  </si>
+  <si>
+    <t>Dragon Bite</t>
+  </si>
+  <si>
+    <t>Ability 1</t>
+  </si>
+  <si>
+    <t>Glaring Shield</t>
+  </si>
+  <si>
+    <t>Ability 1 DMG/HEAL</t>
+  </si>
+  <si>
+    <t>Ability 2</t>
+  </si>
+  <si>
+    <t>Ability 2 DMG/HEAL</t>
+  </si>
+  <si>
+    <t>Ability 3</t>
+  </si>
+  <si>
+    <t>Ability 3 DMG/HEAL</t>
+  </si>
+  <si>
+    <t>Attack</t>
+  </si>
+  <si>
+    <t>defence</t>
+  </si>
+  <si>
+    <t>paralyze</t>
+  </si>
+  <si>
+    <t>Note: Stronger attack cost 2EP,  stronger Def cost 1EP, damging effect cost 2EP(paralyze as well), cure costs 2EP, Heal cost nothing. If offensive, For every extra ability +1. example dragon bite costs 8EP (2+2+2+1+1)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,16 +197,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -255,11 +308,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -278,6 +370,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -299,6 +403,167 @@
         </bottom>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -329,167 +594,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -504,21 +608,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I1048576" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="10" tableBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I1048576" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="9" tableBorderDxfId="10">
   <autoFilter ref="A1:I1048576"/>
   <sortState ref="A2:I1048576">
     <sortCondition ref="A1:A1048576"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="9" name="#" dataDxfId="0"/>
-    <tableColumn id="1" name="Card Name" dataDxfId="9"/>
-    <tableColumn id="2" name="Card type" dataDxfId="8"/>
-    <tableColumn id="3" name="EP" dataDxfId="7"/>
-    <tableColumn id="4" name="EPD" dataDxfId="6"/>
-    <tableColumn id="5" name="EPP" dataDxfId="5"/>
-    <tableColumn id="6" name="Effect" dataDxfId="4"/>
-    <tableColumn id="7" name="Effect DMG" dataDxfId="3"/>
-    <tableColumn id="8" name="Effect Heal" dataDxfId="2"/>
+    <tableColumn id="9" name="#" dataDxfId="8"/>
+    <tableColumn id="1" name="Card Name" dataDxfId="7"/>
+    <tableColumn id="2" name="Card type" dataDxfId="6"/>
+    <tableColumn id="3" name="EP" dataDxfId="5"/>
+    <tableColumn id="4" name="EPD" dataDxfId="4"/>
+    <tableColumn id="5" name="EPP" dataDxfId="3"/>
+    <tableColumn id="6" name="Effect" dataDxfId="2"/>
+    <tableColumn id="7" name="Effect DMG" dataDxfId="1"/>
+    <tableColumn id="8" name="Effect Heal" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -787,10 +891,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1048576"/>
+  <dimension ref="A1:P1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A40"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -803,9 +907,10 @@
     <col min="7" max="7" width="15" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.375" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5" style="2" customWidth="1"/>
+    <col min="11" max="11" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>36</v>
       </c>
@@ -834,7 +939,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -862,8 +967,17 @@
       <c r="I2" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -891,8 +1005,15 @@
       <c r="I3" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3" s="10"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -920,8 +1041,15 @@
       <c r="I4" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4" s="10"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -950,7 +1078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -979,7 +1107,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1008,7 +1136,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1037,7 +1165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1066,7 +1194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1095,7 +1223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1124,7 +1252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1153,7 +1281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1182,7 +1310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1211,7 +1339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1237,7 +1365,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1314,7 +1442,7 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1551,10 +1679,203 @@
       <c r="I1048576" s="7"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="J2:P4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="1.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="1.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="1.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>